<commit_message>
identifiers for org, pract, patient...
</commit_message>
<xml_diff>
--- a/ValueSet-arf-diagnosis-vs.xlsx
+++ b/ValueSet-arf-diagnosis-vs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Property</t>
   </si>
@@ -57,19 +57,25 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-20T12:15:26+10:00</t>
+    <t>2024-05-20T17:01:27+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
   </si>
   <si>
-    <t>Northern Australia Regional Digital Health Collaborative</t>
+    <t>D Foulkes - Northern Australia Regional Digital Health Collaborative</t>
   </si>
   <si>
     <t>Contact</t>
   </si>
   <si>
-    <t>Northern Australia Regional Digital Health Collaborative (https://nardhc.org)</t>
+    <t>D Foulkes - Northern Australia Regional Digital Health Collaborative (https://nardhc.org)</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>Australia</t>
   </si>
   <si>
     <t>Description</t>
@@ -254,7 +260,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -347,27 +353,35 @@
         <v>19</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s" s="2">
         <v>23</v>
+      </c>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -389,58 +403,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added experimental to vs
</commit_message>
<xml_diff>
--- a/ValueSet-arf-diagnosis-vs.xlsx
+++ b/ValueSet-arf-diagnosis-vs.xlsx
@@ -7,13 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from SNOWMED CT" r:id="rId4" sheetId="2"/>
+    <sheet name="Include from SNOMED CT" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Property</t>
   </si>
@@ -54,10 +54,13 @@
     <t>Experimental</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-23T14:45:45+10:00</t>
+    <t>2024-05-23T15:19:20+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -322,43 +325,45 @@
       <c r="A7" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s" s="2">
         <v>9</v>
@@ -366,22 +371,22 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -403,58 +408,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>